<commit_message>
final de controladores, unificacion busqueda en cada controlador
</commit_message>
<xml_diff>
--- a/database/Seguimiento.xlsx
+++ b/database/Seguimiento.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="127">
   <si>
     <t>Colciencias</t>
   </si>
@@ -342,13 +342,76 @@
   </si>
   <si>
     <t>Revisar Ln 437 de mdl_planeacion</t>
+  </si>
+  <si>
+    <t>Clases de producto</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/claProductos.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/tipProductos.php</t>
+  </si>
+  <si>
+    <t>No muestra busqueda de servicios, general ni especifico /hace falta eliminar y modificar (no esta definido )</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/proyecto.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/estProyecto.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/etaProyecto.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/tipProyecto.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/estSolicitud.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/solicitudEspecifica.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/solicitudInicial.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/tipSolicitud.php</t>
+  </si>
+  <si>
+    <t>revisar si a la hora de actualizar lod dos campos no son obligatorios</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/cargo.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/equipo.php</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/password.php</t>
+  </si>
+  <si>
+    <t>el campo ususaio* aparece el codigo html no etsa definida var4</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/perfil.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/usuario.php</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/salarios.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +448,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -394,7 +464,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -478,21 +548,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -618,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -630,40 +685,54 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -945,11 +1014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:K95"/>
+  <dimension ref="D1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,58 +1026,58 @@
     <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="9" max="9" width="69.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D2" s="16" t="s">
+    <row r="2" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="18" t="s">
+      <c r="E2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="29" t="s">
+      <c r="J2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1031,15 +1100,15 @@
       <c r="I3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="27" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1057,15 +1126,15 @@
       <c r="I4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="27" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1083,10 +1152,10 @@
       <c r="I5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="29" t="s">
+      <c r="J5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1109,13 +1178,13 @@
       <c r="I6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="9" t="s">
+      <c r="J6" s="21"/>
+      <c r="K6" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1131,15 +1200,15 @@
       <c r="I7" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="29" t="s">
+      <c r="J7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="26" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>71</v>
       </c>
       <c r="E8" s="2"/>
@@ -1149,10 +1218,10 @@
       <c r="I8" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="29" t="s">
+      <c r="J8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="26" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1178,12 +1247,12 @@
       <c r="J9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1204,12 +1273,12 @@
       <c r="J10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1230,12 +1299,12 @@
       <c r="J11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1256,12 +1325,12 @@
       <c r="J12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1282,12 +1351,12 @@
       <c r="J13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1308,7 +1377,7 @@
       <c r="J14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="29" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1334,12 +1403,12 @@
       <c r="J15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1357,15 +1426,15 @@
       <c r="I16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J16" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="29" t="s">
+      <c r="J16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="26" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1383,15 +1452,15 @@
       <c r="I17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K17" s="29" t="s">
+      <c r="J17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="12" t="s">
+    <row r="18" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1406,13 +1475,13 @@
       <c r="H18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="32" t="s">
         <v>48</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="26" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1420,22 +1489,22 @@
       <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="30" t="s">
+      <c r="E19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K19" s="30" t="s">
@@ -1443,25 +1512,25 @@
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J20" s="30" t="s">
+      <c r="E20" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K20" s="30" t="s">
@@ -1469,25 +1538,25 @@
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J21" s="30" t="s">
+      <c r="E21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K21" s="30" t="s">
@@ -1495,25 +1564,25 @@
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J22" s="30" t="s">
+      <c r="E22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K22" s="30" t="s">
@@ -1521,25 +1590,25 @@
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J23" s="30" t="s">
+      <c r="E23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K23" s="30" t="s">
@@ -1547,25 +1616,25 @@
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J24" s="30" t="s">
+      <c r="E24" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K24" s="30" t="s">
@@ -1573,25 +1642,25 @@
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J25" s="30" t="s">
+      <c r="E25" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K25" s="30" t="s">
@@ -1599,25 +1668,25 @@
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J26" s="30" t="s">
+      <c r="E26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K26" s="30" t="s">
@@ -1625,25 +1694,25 @@
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H27" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J27" s="30" t="s">
+      <c r="E27" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K27" s="30" t="s">
@@ -1651,25 +1720,25 @@
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J28" s="30" t="s">
+      <c r="E28" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K28" s="30" t="s">
@@ -1677,25 +1746,25 @@
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J29" s="30" t="s">
+      <c r="E29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K29" s="30" t="s">
@@ -1703,25 +1772,25 @@
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J30" s="30" t="s">
+      <c r="E30" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K30" s="30" t="s">
@@ -1729,25 +1798,25 @@
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J31" s="30" t="s">
+      <c r="E31" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" s="25" t="s">
         <v>89</v>
       </c>
       <c r="K31" s="30" t="s">
@@ -1776,7 +1845,7 @@
       <c r="J32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="29" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1802,12 +1871,12 @@
       <c r="J33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="K33" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -1825,15 +1894,15 @@
       <c r="I34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J34" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="K34" s="29" t="s">
+      <c r="J34" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="26" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1854,12 +1923,12 @@
       <c r="J35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K35" s="29" t="s">
+      <c r="K35" s="26" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -1877,15 +1946,15 @@
       <c r="I36" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J36" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K36" s="29" t="s">
+      <c r="J36" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" s="26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="10" t="s">
+    <row r="37" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1903,15 +1972,15 @@
       <c r="I37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J37" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K37" s="29" t="s">
+      <c r="J37" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K37" s="26" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1929,15 +1998,15 @@
       <c r="I38" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J38" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K38" s="29" t="s">
+      <c r="J38" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38" s="26" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1955,15 +2024,15 @@
       <c r="I39" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J39" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K39" s="29" t="s">
+      <c r="J39" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K39" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="10" t="s">
+    <row r="40" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D40" s="8" t="s">
         <v>64</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1979,15 +2048,15 @@
         <v>37</v>
       </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K40" s="29" t="s">
+      <c r="J40" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K40" s="26" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -2005,15 +2074,15 @@
       <c r="I41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J41" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K41" s="29" t="s">
+      <c r="J41" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K41" s="26" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -2031,10 +2100,10 @@
       <c r="I42" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J42" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K42" s="29" t="s">
+      <c r="J42" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" s="26" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2060,12 +2129,12 @@
       <c r="J43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="K43" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="8" t="s">
         <v>67</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -2083,15 +2152,15 @@
       <c r="I44" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J44" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K44" s="29" t="s">
+      <c r="J44" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K44" s="26" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="8" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -2109,15 +2178,15 @@
       <c r="I45" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J45" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K45" s="29" t="s">
+      <c r="J45" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K45" s="26" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="8" t="s">
         <v>69</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -2135,10 +2204,10 @@
       <c r="I46" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J46" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K46" s="29" t="s">
+      <c r="J46" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K46" s="26" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2164,291 +2233,654 @@
       <c r="J47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="K47" s="29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="48" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="11"/>
+      <c r="E48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K48" s="29" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="11"/>
+      <c r="E49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K49" s="29" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="11"/>
+      <c r="E50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K50" s="29" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J51" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="11"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D52" s="10" t="s">
+      <c r="E52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K52" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="11"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D53" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="11"/>
+      <c r="I53" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J53" s="22"/>
+      <c r="K53" s="29"/>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K54" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D55" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="11"/>
-    </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D55" s="10" t="s">
+      <c r="E55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K55" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="11"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D56" s="10" t="s">
+      <c r="E56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J56" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K56" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="11"/>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D57" s="10" t="s">
+      <c r="E57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J57" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K57" s="26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="11"/>
-    </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="10" t="s">
+      <c r="E58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J58" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K58" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D59" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="11"/>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D59" s="6" t="s">
+      <c r="E59" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J59" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K59" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D60" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="11"/>
-    </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D60" s="10" t="s">
+      <c r="E60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K60" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D61" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="26"/>
-      <c r="K60" s="11"/>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D61" s="10" t="s">
+      <c r="E61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J61" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K61" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D62" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="11"/>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D62" s="10" t="s">
+      <c r="E62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J62" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K62" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="D63" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="11"/>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D63" s="10" t="s">
+      <c r="E63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J63" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K63" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D64" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="11"/>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D64" s="6" t="s">
+      <c r="E64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J64" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K64" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="26"/>
-      <c r="K64" s="11"/>
-    </row>
-    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D65" s="10" t="s">
+      <c r="E65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="11"/>
-    </row>
-    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D66" s="10" t="s">
+      <c r="E66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J66" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K66" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="26"/>
-      <c r="K66" s="11"/>
-    </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D67" s="10" t="s">
+      <c r="E67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J67" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K67" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D68" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J68" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K68" s="26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D69" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="11"/>
-    </row>
-    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D68" s="10" t="s">
+      <c r="E69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J69" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K69" s="26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D70" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="11"/>
-    </row>
-    <row r="69" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="13" t="s">
+      <c r="E70" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J70" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K70" s="26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D71" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="15"/>
-    </row>
-    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D80" s="1"/>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="1"/>
-    </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="1"/>
+      <c r="E71" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J71" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="K71" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K72" s="31"/>
+    </row>
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="31"/>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="31"/>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K75" s="31"/>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="31"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="1"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="1"/>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="1"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="1"/>
-    </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="1"/>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="1"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="1"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2471,8 +2903,24 @@
     <hyperlink ref="K44" r:id="rId17"/>
     <hyperlink ref="K45" r:id="rId18"/>
     <hyperlink ref="K46" r:id="rId19"/>
+    <hyperlink ref="K51" r:id="rId20"/>
+    <hyperlink ref="K54" r:id="rId21"/>
+    <hyperlink ref="K56" r:id="rId22"/>
+    <hyperlink ref="K57" r:id="rId23"/>
+    <hyperlink ref="K58" r:id="rId24"/>
+    <hyperlink ref="K59" r:id="rId25"/>
+    <hyperlink ref="K61" r:id="rId26"/>
+    <hyperlink ref="K62" r:id="rId27"/>
+    <hyperlink ref="K63" r:id="rId28"/>
+    <hyperlink ref="K64" r:id="rId29"/>
+    <hyperlink ref="K66" r:id="rId30"/>
+    <hyperlink ref="K67" r:id="rId31"/>
+    <hyperlink ref="K68" r:id="rId32"/>
+    <hyperlink ref="K70" r:id="rId33"/>
+    <hyperlink ref="K69" r:id="rId34"/>
+    <hyperlink ref="K71" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Alineacion de tablas a la izquierda
</commit_message>
<xml_diff>
--- a/database/Seguimiento.xlsx
+++ b/database/Seguimiento.xlsx
@@ -266,12 +266,6 @@
     <t>novedad/daño</t>
   </si>
   <si>
-    <t>En la busqueda aparece varias vaeces el numero de pagina, y si no hay resultados sigue mostrando toda la informacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guarda las nuevas cotizaciones pero no las edita, aparece error al asignar personas antes de cotizar  </t>
-  </si>
-  <si>
     <t>http://localhost/sigpys/Views/entidad.php</t>
   </si>
   <si>
@@ -405,6 +399,12 @@
   </si>
   <si>
     <t>http://localhost/sigpys/Views/salarios.php</t>
+  </si>
+  <si>
+    <t>En la busqueda aparece varias vaeces el numero de pagina, y si no hay resultados sigue mostrando toda la informacion // no se actualizo la tabla de buscar (boton editar)</t>
+  </si>
+  <si>
+    <t>Guarda las nuevas cotizaciones pero no las edita, aparece error al asignar personas antes de cotizar   // no se actualizo la tabla de buscar (boton editar)</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1017,8 @@
   <dimension ref="D1:K97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1078,7 @@
         <v>48</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>37</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="4:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11" ht="45" x14ac:dyDescent="0.25">
       <c r="D7" s="8" t="s">
         <v>70</v>
       </c>
@@ -1198,13 +1198,13 @@
         <v>37</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1216,13 +1216,13 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="26" t="s">
         <v>81</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
         <v>48</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>48</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>48</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
@@ -1490,25 +1490,25 @@
         <v>6</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
@@ -1516,25 +1516,25 @@
         <v>16</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
@@ -1542,25 +1542,25 @@
         <v>17</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K21" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
@@ -1568,25 +1568,25 @@
         <v>32</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K22" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
@@ -1594,25 +1594,25 @@
         <v>18</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
@@ -1620,25 +1620,25 @@
         <v>33</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
@@ -1646,25 +1646,25 @@
         <v>34</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
@@ -1672,25 +1672,25 @@
         <v>35</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
@@ -1698,25 +1698,25 @@
         <v>36</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
@@ -1724,25 +1724,25 @@
         <v>19</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K28" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
@@ -1750,25 +1750,25 @@
         <v>20</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K29" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
@@ -1776,25 +1776,25 @@
         <v>21</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K30" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
@@ -1802,30 +1802,30 @@
         <v>22</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>48</v>
@@ -1892,13 +1892,13 @@
         <v>37</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J34" s="21" t="s">
         <v>37</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
         <v>48</v>
       </c>
       <c r="K35" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
@@ -1944,13 +1944,13 @@
         <v>37</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J36" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K36" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
         <v>48</v>
       </c>
       <c r="K37" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
@@ -1996,13 +1996,13 @@
         <v>37</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J38" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K38" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
@@ -2022,13 +2022,13 @@
         <v>37</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J39" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -2052,7 +2052,7 @@
         <v>48</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
@@ -2072,13 +2072,13 @@
         <v>37</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J41" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K41" s="26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
@@ -2098,13 +2098,13 @@
         <v>37</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K42" s="26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.25">
@@ -2150,13 +2150,13 @@
         <v>37</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J44" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
         <v>48</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
@@ -2202,13 +2202,13 @@
         <v>37</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J46" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K46" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.25">
@@ -2317,7 +2317,7 @@
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>37</v>
@@ -2338,7 +2338,7 @@
         <v>48</v>
       </c>
       <c r="K51" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J53" s="22"/>
       <c r="K53" s="29"/>
@@ -2404,7 +2404,7 @@
         <v>48</v>
       </c>
       <c r="K54" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>48</v>
       </c>
       <c r="K56" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
         <v>48</v>
       </c>
       <c r="K57" s="26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
         <v>48</v>
       </c>
       <c r="K58" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>48</v>
       </c>
       <c r="K59" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="4:11" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
         <v>48</v>
       </c>
       <c r="K61" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>48</v>
       </c>
       <c r="K62" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>48</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="4:11" x14ac:dyDescent="0.25">
@@ -2658,13 +2658,13 @@
         <v>37</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J64" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K64" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="4:11" x14ac:dyDescent="0.25">
@@ -2710,13 +2710,13 @@
         <v>37</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J66" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K66" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="4:11" x14ac:dyDescent="0.25">
@@ -2736,39 +2736,39 @@
         <v>37</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J67" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K67" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D68" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="J68" s="22" t="s">
         <v>37</v>
       </c>
       <c r="K68" s="26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="4:11" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
         <v>48</v>
       </c>
       <c r="K69" s="26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="4:11" x14ac:dyDescent="0.25">
@@ -2814,13 +2814,13 @@
         <v>37</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J70" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K70" s="26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2840,13 +2840,13 @@
         <v>48</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J71" s="23" t="s">
         <v>48</v>
       </c>
       <c r="K71" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Registrar Password, Actualizacion de boton buscar
</commit_message>
<xml_diff>
--- a/database/Seguimiento.xlsx
+++ b/database/Seguimiento.xlsx
@@ -401,17 +401,17 @@
     <t>http://localhost/sigpys/Views/salarios.php</t>
   </si>
   <si>
-    <t>En la busqueda aparece varias vaeces el numero de pagina, y si no hay resultados sigue mostrando toda la informacion // no se actualizo la tabla de buscar (boton editar)</t>
-  </si>
-  <si>
     <t>Guarda las nuevas cotizaciones pero no las edita, aparece error al asignar personas antes de cotizar   // no se actualizo la tabla de buscar (boton editar)</t>
+  </si>
+  <si>
+    <t>En la busqueda aparece varias vaeces el numero de pagina, y si no hay resultados sigue mostrando toda la informacion//  ControladorBuscar/Vista cambio de ctr_bus.. A ctrl_..  // no se actualizo la tabla de buscar (boton editar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,13 +448,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -673,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -732,7 +725,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1183,7 +1175,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="4:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11" ht="60" x14ac:dyDescent="0.25">
       <c r="D7" s="8" t="s">
         <v>70</v>
       </c>
@@ -1198,7 +1190,7 @@
         <v>37</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>37</v>
@@ -1216,7 +1208,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>37</v>
@@ -1475,8 +1467,8 @@
       <c r="H18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="32" t="s">
-        <v>48</v>
+      <c r="I18" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
modificacion vista password y modal de recuperacion de contraseña
</commit_message>
<xml_diff>
--- a/database/Seguimiento.xlsx
+++ b/database/Seguimiento.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="123">
   <si>
     <t>Colciencias</t>
   </si>
@@ -242,9 +242,6 @@
     <t xml:space="preserve">Nueva Cotización </t>
   </si>
   <si>
-    <t>cambio de if(!empty($...){}if(emply($...){}</t>
-  </si>
-  <si>
     <t>Hace falta definir Select Investigador / no dirigue al modal (No se envia la variable "cod2")</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
     <t>Inventario</t>
   </si>
   <si>
-    <t xml:space="preserve">El select de coordinadores (registrar) muestra el nombre doble </t>
-  </si>
-  <si>
     <t>http://localhost/SIGPYS/Views/celula.php</t>
   </si>
   <si>
@@ -347,9 +341,6 @@
     <t>http://localhost/sigpys/Views/tipProductos.php</t>
   </si>
   <si>
-    <t>No muestra busqueda de servicios, general ni especifico /hace falta eliminar y modificar (no esta definido )</t>
-  </si>
-  <si>
     <t>http://localhost/sigpys/Views/proyecto.php</t>
   </si>
   <si>
@@ -374,9 +365,6 @@
     <t>http://localhost/sigpys/Views/tipSolicitud.php</t>
   </si>
   <si>
-    <t>revisar si a la hora de actualizar lod dos campos no son obligatorios</t>
-  </si>
-  <si>
     <t>http://localhost/sigpys/Views/cargo.php</t>
   </si>
   <si>
@@ -389,9 +377,6 @@
     <t>http://localhost/sigpys/Views/password.php</t>
   </si>
   <si>
-    <t>el campo ususaio* aparece el codigo html no etsa definida var4</t>
-  </si>
-  <si>
     <t>http://localhost/sigpys/Views/perfil.php</t>
   </si>
   <si>
@@ -405,6 +390,9 @@
   </si>
   <si>
     <t>En la busqueda aparece varias vaeces el numero de pagina, y si no hay resultados sigue mostrando toda la informacion//  ControladorBuscar/Vista cambio de ctr_bus.. A ctrl_..  // no se actualizo la tabla de buscar (boton editar)</t>
+  </si>
+  <si>
+    <t>http://localhost/sigpys/Views/servicios.php</t>
   </si>
 </sst>
 </file>
@@ -666,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -725,6 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1010,7 +999,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,10 +1012,10 @@
   <sheetData>
     <row r="1" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>38</v>
@@ -1041,15 +1030,15 @@
         <v>41</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D2" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>37</v>
@@ -1063,14 +1052,12 @@
       <c r="H2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="I2" s="14"/>
       <c r="J2" s="19" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
@@ -1122,7 +1109,7 @@
         <v>48</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1142,13 +1129,13 @@
         <v>48</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
@@ -1190,13 +1177,13 @@
         <v>37</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1208,13 +1195,13 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>37</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
@@ -1422,7 +1409,7 @@
         <v>48</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
@@ -1448,7 +1435,7 @@
         <v>48</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1468,13 +1455,13 @@
         <v>37</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
@@ -1482,25 +1469,25 @@
         <v>6</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
@@ -1508,25 +1495,25 @@
         <v>16</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
@@ -1534,25 +1521,25 @@
         <v>17</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K21" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
@@ -1560,25 +1547,25 @@
         <v>32</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K22" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
@@ -1586,25 +1573,25 @@
         <v>18</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
@@ -1612,25 +1599,25 @@
         <v>33</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
@@ -1638,25 +1625,25 @@
         <v>34</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
@@ -1664,25 +1651,25 @@
         <v>35</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
@@ -1690,25 +1677,25 @@
         <v>36</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
@@ -1716,25 +1703,25 @@
         <v>19</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K28" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
@@ -1742,25 +1729,25 @@
         <v>20</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K29" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
@@ -1768,25 +1755,25 @@
         <v>21</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K30" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
@@ -1794,30 +1781,30 @@
         <v>22</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>48</v>
@@ -1883,14 +1870,12 @@
       <c r="H34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>89</v>
-      </c>
+      <c r="I34" s="2"/>
       <c r="J34" s="21" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
@@ -1916,7 +1901,7 @@
         <v>48</v>
       </c>
       <c r="K35" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
@@ -1936,13 +1921,13 @@
         <v>37</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J36" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K36" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -1968,7 +1953,7 @@
         <v>48</v>
       </c>
       <c r="K37" s="26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
@@ -1988,13 +1973,13 @@
         <v>37</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J38" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K38" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
@@ -2014,13 +1999,13 @@
         <v>37</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J39" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -2044,7 +2029,7 @@
         <v>48</v>
       </c>
       <c r="K40" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
@@ -2064,13 +2049,13 @@
         <v>37</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J41" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K41" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
@@ -2090,13 +2075,13 @@
         <v>37</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J42" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K42" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.25">
@@ -2142,13 +2127,13 @@
         <v>37</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J44" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K44" s="26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
@@ -2174,7 +2159,7 @@
         <v>48</v>
       </c>
       <c r="K45" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
@@ -2194,13 +2179,13 @@
         <v>37</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J46" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K46" s="26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.25">
@@ -2309,7 +2294,7 @@
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>37</v>
@@ -2330,7 +2315,7 @@
         <v>48</v>
       </c>
       <c r="K51" s="26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
@@ -2363,15 +2348,27 @@
       <c r="D53" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
+      <c r="E53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="I53" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J53" s="22"/>
-      <c r="K53" s="29"/>
+        <v>48</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K53" s="32" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" s="8" t="s">
@@ -2396,7 +2393,7 @@
         <v>48</v>
       </c>
       <c r="K54" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.25">
@@ -2448,7 +2445,7 @@
         <v>48</v>
       </c>
       <c r="K56" s="26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
@@ -2474,7 +2471,7 @@
         <v>48</v>
       </c>
       <c r="K57" s="26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.25">
@@ -2500,7 +2497,7 @@
         <v>48</v>
       </c>
       <c r="K58" s="26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.25">
@@ -2526,7 +2523,7 @@
         <v>48</v>
       </c>
       <c r="K59" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="4:11" x14ac:dyDescent="0.25">
@@ -2578,7 +2575,7 @@
         <v>48</v>
       </c>
       <c r="K61" s="26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -2604,7 +2601,7 @@
         <v>48</v>
       </c>
       <c r="K62" s="26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="4:11" ht="30" x14ac:dyDescent="0.25">
@@ -2630,7 +2627,7 @@
         <v>48</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="4:11" x14ac:dyDescent="0.25">
@@ -2650,13 +2647,13 @@
         <v>37</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="J64" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K64" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="4:11" x14ac:dyDescent="0.25">
@@ -2702,13 +2699,13 @@
         <v>37</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J66" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K66" s="26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="4:11" x14ac:dyDescent="0.25">
@@ -2728,39 +2725,39 @@
         <v>37</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J67" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K67" s="26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D68" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="J68" s="22" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K68" s="26" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="4:11" x14ac:dyDescent="0.25">
@@ -2786,7 +2783,7 @@
         <v>48</v>
       </c>
       <c r="K69" s="26" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="4:11" x14ac:dyDescent="0.25">
@@ -2806,39 +2803,39 @@
         <v>37</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J70" s="22" t="s">
         <v>48</v>
       </c>
       <c r="K70" s="26" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D71" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E71" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G71" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H71" s="11" t="s">
-        <v>48</v>
+      <c r="E71" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J71" s="23" t="s">
         <v>48</v>
       </c>
       <c r="K71" s="26" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="4:11" x14ac:dyDescent="0.25">
@@ -2911,8 +2908,9 @@
     <hyperlink ref="K70" r:id="rId33"/>
     <hyperlink ref="K69" r:id="rId34"/>
     <hyperlink ref="K71" r:id="rId35"/>
+    <hyperlink ref="K53" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>